<commit_message>
-movie scraping to exel file
</commit_message>
<xml_diff>
--- a/week3/prac01.xlsx
+++ b/week3/prac01.xlsx
@@ -12,18 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
-    <t>번호</t>
+    <t>랭킹</t>
   </si>
   <si>
     <t>이름</t>
   </si>
   <si>
-    <t>성적</t>
-  </si>
-  <si>
-    <t>상위권</t>
+    <t>별점</t>
   </si>
 </sst>
 </file>
@@ -1341,9 +1338,7 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
-        <v>3</v>
-      </c>
+      <c r="D1" s="2"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>

</xml_diff>